<commit_message>
Added BE W9 and W10
</commit_message>
<xml_diff>
--- a/data/spss_files_be.xlsx
+++ b/data/spss_files_be.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kw\Documents\comix_data_clean\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F546F531-EBF3-414F-9629-6E2DDAF21FA3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D5B6C6A-7204-4B77-9D23-843B56377B23}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="5" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="39">
   <si>
     <t>country</t>
   </si>
@@ -149,6 +149,9 @@
   </si>
   <si>
     <t>20_060765_BE2_Wave9_Final_v1_150321_IntClientUse</t>
+  </si>
+  <si>
+    <t>21-019042_BE_Wave10_Final_v1_260321_IntClientUse</t>
   </si>
 </sst>
 </file>
@@ -481,14 +484,14 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8203125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -496,7 +499,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -504,7 +507,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -512,7 +515,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -520,7 +523,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -528,7 +531,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
@@ -543,24 +546,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C042354-CAAB-48AD-AFC2-2197A2D12C9D}">
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8203125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.29296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.29296875" customWidth="1"/>
-    <col min="4" max="4" width="12.234375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.46875" customWidth="1"/>
-    <col min="8" max="8" width="58.46875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.46875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
+    <col min="8" max="8" width="58.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -604,7 +607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -637,7 +640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -663,14 +666,14 @@
         <v>14</v>
       </c>
       <c r="I3" s="2" t="str">
-        <f t="shared" ref="I3:I18" si="0">A3&amp;"_"&amp;"sr"&amp;TEXT(D3,"00")&amp;"_"&amp;YEAR(G3)&amp;TEXT(G3,"MM")&amp;TEXT(G3,"DD")&amp;"_p"&amp;E3&amp;"_wv"&amp;TEXT(F3,"00")&amp;""</f>
+        <f t="shared" ref="I3:I19" si="0">A3&amp;"_"&amp;"sr"&amp;TEXT(D3,"00")&amp;"_"&amp;YEAR(G3)&amp;TEXT(G3,"MM")&amp;TEXT(G3,"DD")&amp;"_p"&amp;E3&amp;"_wv"&amp;TEXT(F3,"00")&amp;""</f>
         <v>be_sr02_20200518_pA_wv02</v>
       </c>
       <c r="J3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -703,7 +706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -736,7 +739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -769,7 +772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -802,7 +805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -835,7 +838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -868,7 +871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
@@ -894,7 +897,7 @@
         <v>be_sr09_20201120_pB_wv01</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -918,7 +921,7 @@
         <v>be_sr10_19000100_pB_wv02</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -942,7 +945,7 @@
         <v>be_sr11_19000100_pB_wv03</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -972,7 +975,7 @@
         <v>be_sr12_20210111_pB_wv04</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -1002,7 +1005,7 @@
         <v>be_sr13_20210120_pB_wv05</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
@@ -1032,7 +1035,7 @@
         <v>be_sr14_20210127_pB_wv06</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -1062,7 +1065,7 @@
         <v>be_sr15_20210222_pB_wv07</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>12</v>
       </c>
@@ -1092,7 +1095,7 @@
         <v>be_sr16_20210226_pB_wv08</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -1120,6 +1123,36 @@
       <c r="I18" t="str">
         <f t="shared" si="0"/>
         <v>be_sr17_20210316_pB_wv09</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19">
+        <v>5</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>18</v>
+      </c>
+      <c r="E19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19">
+        <v>10</v>
+      </c>
+      <c r="G19" s="3">
+        <v>44285</v>
+      </c>
+      <c r="H19" t="s">
+        <v>38</v>
+      </c>
+      <c r="I19" t="str">
+        <f t="shared" si="0"/>
+        <v>be_sr18_20210330_pB_wv10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>